<commit_message>
lots of item, synergy, blessing progress
</commit_message>
<xml_diff>
--- a/notes/Items.xlsx
+++ b/notes/Items.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/858ebd3f783c0785/AdventureGame/notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/858ebd3f783c0785/AdventureGame_MUD_ECS/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{6CBA61C9-C556-4C8D-822C-179E6D506B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9360B7D-EC6E-434E-ACD5-B28789652B81}"/>
+  <xr:revisionPtr revIDLastSave="520" documentId="8_{6CBA61C9-C556-4C8D-822C-179E6D506B48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0FD969E7-2729-4477-93A8-7EAE10B7AFAD}"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="3900" windowWidth="26040" windowHeight="17310" xr2:uid="{7A78DAEA-021F-48C2-A4E4-C77CB8C32F89}"/>
+    <workbookView xWindow="12720" yWindow="555" windowWidth="28215" windowHeight="20040" xr2:uid="{7A78DAEA-021F-48C2-A4E4-C77CB8C32F89}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
     <sheet name="Armor" sheetId="2" r:id="rId2"/>
-    <sheet name="Tributes" sheetId="3" r:id="rId3"/>
+    <sheet name="Synergies" sheetId="3" r:id="rId3"/>
+    <sheet name="Blessings" sheetId="4" r:id="rId4"/>
+    <sheet name="Items" sheetId="5" r:id="rId5"/>
+    <sheet name="Components" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="166">
   <si>
     <t>Weapons</t>
   </si>
@@ -68,9 +71,6 @@
     <t>Effect</t>
   </si>
   <si>
-    <t>Buckler</t>
-  </si>
-  <si>
     <t>Offhand</t>
   </si>
   <si>
@@ -80,9 +80,6 @@
     <t>Head</t>
   </si>
   <si>
-    <t>Clogs</t>
-  </si>
-  <si>
     <t>Footwraps</t>
   </si>
   <si>
@@ -101,21 +98,12 @@
     <t>NimbleGod</t>
   </si>
   <si>
-    <t>Tributes</t>
-  </si>
-  <si>
     <t>+1 Agility</t>
   </si>
   <si>
-    <t>ChadGod</t>
-  </si>
-  <si>
     <t>+1 Strength</t>
   </si>
   <si>
-    <t>GodGod</t>
-  </si>
-  <si>
     <t>+1 Intelligence</t>
   </si>
   <si>
@@ -146,9 +134,6 @@
     <t>Light</t>
   </si>
   <si>
-    <t>+1 damage if your strength is greater than the opponent's. '+1 damage if your agility is greater than the opponent's</t>
-  </si>
-  <si>
     <t>Dagger</t>
   </si>
   <si>
@@ -197,27 +182,15 @@
     <t>No</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>On hit: 25% chance to stun opponent for 2 turns</t>
   </si>
   <si>
-    <t>On first hit: Heal 1</t>
-  </si>
-  <si>
     <t>+50% dodge chance against first non-natural attack on you</t>
   </si>
   <si>
-    <t>+1 damage against opponents using natural attack</t>
-  </si>
-  <si>
     <t>Great Sword</t>
   </si>
   <si>
-    <t>Very Rare</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -231,13 +204,343 @@
   </si>
   <si>
     <t>A damp cloth. Smells like chemicals.</t>
+  </si>
+  <si>
+    <t>+1 damage against opponents using natural weapon</t>
+  </si>
+  <si>
+    <t>Crit: Does +1 damage</t>
+  </si>
+  <si>
+    <t>30% chance to do 1 extra damage</t>
+  </si>
+  <si>
+    <t>Rapier</t>
+  </si>
+  <si>
+    <t>Nullify the opponent's chest armor</t>
+  </si>
+  <si>
+    <t>+1 damage if your strength is greater than the opponent's. +1 damage if your agility is greater than the opponent's</t>
+  </si>
+  <si>
+    <t>Gaia</t>
+  </si>
+  <si>
+    <t>Start combat boosted</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Charismatic dialogue options</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>Wise</t>
+  </si>
+  <si>
+    <t>boosted</t>
+  </si>
+  <si>
+    <t>healthy</t>
+  </si>
+  <si>
+    <t>wounded</t>
+  </si>
+  <si>
+    <t>Synergy</t>
+  </si>
+  <si>
+    <t>Always take the first turn</t>
+  </si>
+  <si>
+    <t>God</t>
+  </si>
+  <si>
+    <t>Davebot</t>
+  </si>
+  <si>
+    <t>Prevent first death. Then grants -1 str</t>
+  </si>
+  <si>
+    <t>5 gold</t>
+  </si>
+  <si>
+    <t>Random Uncommon Item</t>
+  </si>
+  <si>
+    <t>8 gold</t>
+  </si>
+  <si>
+    <t>30 gold</t>
+  </si>
+  <si>
+    <t>Random Rare item</t>
+  </si>
+  <si>
+    <t>Random Common item</t>
+  </si>
+  <si>
+    <t>Reduce shop costs by ????%</t>
+  </si>
+  <si>
+    <t>Health potion</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Stuns enemy for 2 turns</t>
+  </si>
+  <si>
+    <t>10 gold</t>
+  </si>
+  <si>
+    <t>Heal 1</t>
+  </si>
+  <si>
+    <t>Stun Grenade</t>
+  </si>
+  <si>
+    <t>15 gold</t>
+  </si>
+  <si>
+    <t>Cure All</t>
+  </si>
+  <si>
+    <t>50 gold</t>
+  </si>
+  <si>
+    <t>Max heal</t>
+  </si>
+  <si>
+    <t>Health boost</t>
+  </si>
+  <si>
+    <t>Antidote</t>
+  </si>
+  <si>
+    <t>Cures poison</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>Cures mute</t>
+  </si>
+  <si>
+    <t>Humans</t>
+  </si>
+  <si>
+    <t>Rats</t>
+  </si>
+  <si>
+    <t>Gods</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Tower Shield</t>
+  </si>
+  <si>
+    <t>Plate Cuirass</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Reduce non-natural attacks by 1 damage (min 1)</t>
+  </si>
+  <si>
+    <t>Holy Guantlets</t>
+  </si>
+  <si>
+    <t>Hands</t>
+  </si>
+  <si>
+    <t>Reduce natural attacks to 1 damage</t>
+  </si>
+  <si>
+    <t>holy</t>
+  </si>
+  <si>
+    <t>arcane</t>
+  </si>
+  <si>
+    <t>Reduce arcane damage by 1</t>
+  </si>
+  <si>
+    <t>Shrunken Head</t>
+  </si>
+  <si>
+    <t>Trinket</t>
+  </si>
+  <si>
+    <t>Reduce holy damage by 1</t>
+  </si>
+  <si>
+    <t>Chest Guard</t>
+  </si>
+  <si>
+    <t>Brawler</t>
+  </si>
+  <si>
+    <t>Scrappy</t>
+  </si>
+  <si>
+    <t>Improved drop chance</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Rogue</t>
+  </si>
+  <si>
+    <t>Your attack damage can't be reduced</t>
+  </si>
+  <si>
+    <t>Longbow</t>
+  </si>
+  <si>
+    <t>Free attack at start of combat</t>
+  </si>
+  <si>
+    <t>Round Shield</t>
+  </si>
+  <si>
+    <t>50% chance to block. Works once per combat</t>
+  </si>
+  <si>
+    <t>Kite Shield</t>
+  </si>
+  <si>
+    <t>50% chance to block. Works twice per combat</t>
+  </si>
+  <si>
+    <t>PBRmor</t>
+  </si>
+  <si>
+    <t>Resist poison and mute effects</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>Pot Lid</t>
+  </si>
+  <si>
+    <t>Sandals</t>
+  </si>
+  <si>
+    <t>Feet</t>
+  </si>
+  <si>
+    <t>See enemy stats</t>
+  </si>
+  <si>
+    <t>Resist mute</t>
+  </si>
+  <si>
+    <t>Ankh</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>Wounded</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Healthy+</t>
+  </si>
+  <si>
+    <t>Healthy++</t>
+  </si>
+  <si>
+    <t>Healthy+++</t>
+  </si>
+  <si>
+    <t>Heal 1. Can heal to Healthy+</t>
+  </si>
+  <si>
+    <t>Heal to Healthy</t>
+  </si>
+  <si>
+    <t>Heal to Healthy+. Remove negative statuses</t>
+  </si>
+  <si>
+    <t>Consumed on death. Respawn in the Rat Manor as Rat Overlord at RatHealthyVoodooBoosted++</t>
+  </si>
+  <si>
+    <t>On first hit: Heal 1. Up to Healthy+</t>
+  </si>
+  <si>
+    <t>Increases heal effect caps by 1</t>
+  </si>
+  <si>
+    <t>Vigor</t>
+  </si>
+  <si>
+    <t>Reading Glasses</t>
+  </si>
+  <si>
+    <t>Tiger Mask</t>
+  </si>
+  <si>
+    <t>Tunic</t>
+  </si>
+  <si>
+    <t>Heal 1 on second turn. Up to Healthy+</t>
+  </si>
+  <si>
+    <t>Increase healing cap by 1</t>
+  </si>
+  <si>
+    <t>+20% chance to crit</t>
+  </si>
+  <si>
+    <t>Super Rare</t>
+  </si>
+  <si>
+    <t>Rail Gun</t>
+  </si>
+  <si>
+    <t>10% chance to insta-gib at start of battle</t>
+  </si>
+  <si>
+    <t>Rabbit's Foot</t>
+  </si>
+  <si>
+    <t>Sorcerer's Ring</t>
+  </si>
+  <si>
+    <t>Amulet of Power</t>
+  </si>
+  <si>
+    <t>Wedding Ring</t>
+  </si>
+  <si>
+    <t>Whetstone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,7 +567,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,7 +575,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="4" tint="0.39997558519241921"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -298,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -306,6 +638,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9844ACED-7881-46C0-B225-0650D470682C}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,8 +967,8 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="104.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="103.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -646,286 +982,370 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>21</v>
+      <c r="F4" t="s">
+        <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>24</v>
+      <c r="F5" t="s">
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>26</v>
+      <c r="F6" t="s">
+        <v>118</v>
       </c>
       <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>55</v>
-      </c>
-      <c r="H6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
+      <c r="F8" t="s">
+        <v>121</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
+      <c r="F9" t="s">
+        <v>151</v>
+      </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
+      <c r="F10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
-      <c r="G11" t="s">
-        <v>46</v>
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15">
         <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>6</v>
       </c>
     </row>
@@ -936,66 +1356,400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B56202A-05AE-4DAF-8E1D-FE1B7022DD78}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="61" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1006,23 +1760,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17E6359-B6C2-43C7-A89A-22620EAC610B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1030,28 +1785,351 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30175D93-74E5-435F-8549-55DD16A0A7CF}">
+  <dimension ref="A3:F32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57154B77-4981-40CF-A011-57DEF7CB63A1}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D033D1F-BDB6-4C5F-9D0B-AA0E12D39C32}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor item changes. combat roller is more intuitive now
</commit_message>
<xml_diff>
--- a/notes/Items.xlsx
+++ b/notes/Items.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\code\adv\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\AdventureGame_MUD_ECS\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C88F0EC-489F-452D-91E7-360CAC9D9DB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12585" activeTab="6"/>
+    <workbookView xWindow="13455" yWindow="1845" windowWidth="10230" windowHeight="16890" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weapons" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <sheet name="Components" sheetId="6" r:id="rId6"/>
     <sheet name="CombatSim" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="204">
   <si>
     <t>Weapons</t>
   </si>
@@ -260,21 +261,12 @@
     <t>5 gold</t>
   </si>
   <si>
-    <t>Random Uncommon Item</t>
-  </si>
-  <si>
     <t>8 gold</t>
   </si>
   <si>
     <t>30 gold</t>
   </si>
   <si>
-    <t>Random Rare item</t>
-  </si>
-  <si>
-    <t>Random Common item</t>
-  </si>
-  <si>
     <t>Reduce shop costs by ????%</t>
   </si>
   <si>
@@ -614,14 +606,56 @@
     <t>X</t>
   </si>
   <si>
-    <t>Click a blank cell and press delete to re-randomize</t>
+    <t>Each player has 50% block and 10% dodge every turn</t>
+  </si>
+  <si>
+    <t>Each player has 50% block/10% dodge 1st turn, then no evasion</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Click the red cell, then press delete to re-randomize</t>
+  </si>
+  <si>
+    <t>Get a random rare item. 1% chance to also get a super rare item</t>
+  </si>
+  <si>
+    <t>Get a random common item. 1% chance to also get an uncommon item</t>
+  </si>
+  <si>
+    <t>Get a random uncommon item. 1% chance to also get a rare item</t>
+  </si>
+  <si>
+    <t>Bronze Crate</t>
+  </si>
+  <si>
+    <t>Silver Crate</t>
+  </si>
+  <si>
+    <t>Gold Crate</t>
+  </si>
+  <si>
+    <t>Mystery Crate</t>
+  </si>
+  <si>
+    <t>Note: Maybe just have the Mystery Crate, not the other crates</t>
+  </si>
+  <si>
+    <t>Odds:</t>
+  </si>
+  <si>
+    <t>Get a random item (common, uncommon, rare, super rare)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -690,6 +724,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -711,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -734,11 +775,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -757,13 +836,31 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1074,7 +1171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1139,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>49</v>
@@ -1165,10 +1262,10 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H4" t="s">
         <v>53</v>
@@ -1191,7 +1288,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
         <v>40</v>
@@ -1217,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
         <v>48</v>
@@ -1243,13 +1340,13 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1269,13 +1366,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1295,13 +1392,13 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G9" t="s">
         <v>40</v>
       </c>
       <c r="H9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1321,13 +1418,13 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1347,13 +1444,13 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1373,13 +1470,13 @@
         <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G12" t="s">
         <v>40</v>
       </c>
       <c r="H12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1399,13 +1496,13 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G13" t="s">
         <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1425,18 +1522,18 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G14" t="s">
         <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -1451,13 +1548,13 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
         <v>117</v>
       </c>
-      <c r="G15" t="s">
-        <v>120</v>
-      </c>
       <c r="H15" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -1501,7 +1598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1542,7 +1639,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>44</v>
@@ -1551,7 +1648,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -1568,7 +1665,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1576,19 +1673,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,27 +1696,27 @@
         <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B8" t="s">
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1627,41 +1724,41 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
         <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
@@ -1670,32 +1767,32 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
         <v>45</v>
@@ -1704,15 +1801,15 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -1721,15 +1818,15 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
         <v>45</v>
@@ -1738,119 +1835,119 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
         <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>20</v>
@@ -1858,13 +1955,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>21</v>
@@ -1872,13 +1969,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>22</v>
@@ -1886,58 +1983,58 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1947,7 +2044,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
@@ -1991,7 +2088,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
         <v>62</v>
@@ -1999,7 +2096,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -2007,41 +2104,41 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2056,12 +2153,12 @@
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2070,7 +2167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2106,7 +2203,7 @@
         <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2114,7 +2211,7 @@
         <v>72</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2122,57 +2219,57 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2181,142 +2278,187 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="21">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="D4" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="22">
+        <v>2E-3</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>91</v>
       </c>
-      <c r="B7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C13" t="s">
-        <v>144</v>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2325,7 +2467,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2336,7 +2478,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2345,11 +2487,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2359,56 +2501,76 @@
     <col min="8" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="H2" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>190</v>
+        <v>187</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>191</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M3" s="11"/>
       <c r="N3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13">
@@ -2418,8 +2580,15 @@
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),3,2)</f>
         <v>2</v>
       </c>
+      <c r="G4" t="str">
+        <f ca="1">IF(LEFT(G3,1)="P",G3,IF(AND(F4=0,G3="-"),"P1 wins",IF(AND(C4=0,G3="-"),"P2 Wins","-")))</f>
+        <v>-</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>191</v>
+      </c>
       <c r="J4" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K4" s="13"/>
       <c r="L4" s="13">
@@ -2428,202 +2597,265 @@
       <c r="M4" s="11"/>
       <c r="O4">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),3,2)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="P4" t="str">
+        <f ca="1">IF(LEFT(P3,1)="P",P3,IF(AND(O4=0,P3="-"),"P1 wins",IF(AND(L4=0,P3="-"),"P2 Wins","-")))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),C4,C4-1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13">
         <f ca="1">F4</f>
         <v>2</v>
       </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G13" ca="1" si="0">IF(LEFT(G4,1)="P",G4,IF(AND(F5=0,G4="-"),"P1 wins",IF(AND(C5=0,G4="-"),"P2 Wins","-")))</f>
+        <v>-</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>192</v>
+      </c>
       <c r="J5" s="11"/>
       <c r="L5">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),L4,L4-1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="13">
         <f ca="1">O4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" ref="P5:P13" ca="1" si="1">IF(LEFT(P4,1)="P",P4,IF(AND(O5=0,P4="-"),"P1 wins",IF(AND(L5=0,P4="-"),"P2 Wins","-")))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="13">
         <f ca="1">C5</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),F4,F4-1)</f>
         <v>1</v>
       </c>
-      <c r="H6" s="15"/>
+      <c r="G6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="H6" s="14"/>
       <c r="J6" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K6" s="13"/>
       <c r="L6" s="13">
         <f ca="1">L5</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="11"/>
       <c r="O6">
         <f ca="1">O5-1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),C6,C6-1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13">
         <f ca="1">F6</f>
         <v>1</v>
       </c>
+      <c r="G7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>-</v>
+      </c>
       <c r="J7" s="11"/>
       <c r="L7">
         <f ca="1">L6-1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="13">
         <f ca="1">O6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13">
         <f ca="1">C7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),F6,F6-1)</f>
         <v>0</v>
       </c>
+      <c r="G8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
+      </c>
       <c r="J8" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13">
         <f ca="1">L7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8" s="11"/>
       <c r="O8">
         <f ca="1">O7-1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),C7,C7-1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13">
         <f ca="1">F8</f>
         <v>0</v>
       </c>
+      <c r="G9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
+      </c>
       <c r="J9" s="11"/>
       <c r="L9">
         <f ca="1">L8-1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="13">
         <f ca="1">O8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13">
         <f ca="1">C9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),F8,F8-1)</f>
         <v>-1</v>
       </c>
+      <c r="G10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
+      </c>
       <c r="J10" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="13">
         <f ca="1">L9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="11"/>
       <c r="O10">
         <f ca="1">O9-1</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C11">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),C9,C9-1)</f>
         <v>0</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13">
         <f ca="1">F10</f>
         <v>-1</v>
       </c>
+      <c r="G11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
+      </c>
       <c r="J11" s="11"/>
       <c r="L11">
         <f ca="1">L10-1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="13">
         <f ca="1">O10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13">
@@ -2632,65 +2864,83 @@
       </c>
       <c r="F12">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),F10,F10-1)</f>
-        <v>-1</v>
+        <v>-2</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13">
         <f ca="1">L11</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M12" s="11"/>
       <c r="O12">
         <f ca="1">O11-1</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13">
         <f ca="1">IF(OR(RAND()&gt;=0.75, RAND()&gt;=0.9),C11,C11-1)</f>
         <v>-1</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13">
         <f ca="1">F12</f>
-        <v>-1</v>
+        <v>-2</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>P1 wins</v>
       </c>
       <c r="J13" s="11"/>
       <c r="L13">
         <f ca="1">L12-1</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N13" s="13"/>
       <c r="O13" s="13">
         <f ca="1">O12</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>-2</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>P1 wins</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
       <c r="J14" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="F1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>